<commit_message>
Accident upload and mapping added
</commit_message>
<xml_diff>
--- a/src/img/traffic_data.xlsx
+++ b/src/img/traffic_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Accident Mapper\src\img\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20D995-9CA6-4CC0-8519-C85369EFA5BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Record Number</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a summary of the first accident data point. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a summary of the second accident data point. </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +359,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="C2">
+        <v>-86.4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>-87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added clear map button
</commit_message>
<xml_diff>
--- a/src/img/traffic_data.xlsx
+++ b/src/img/traffic_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Accident Mapper\src\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\Programming\Web Apps\2019 Accident Map Redesign\src\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F20D995-9CA6-4CC0-8519-C85369EFA5BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2EB70D-31AC-403C-940B-5CDCE6C7EB58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Record Number</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t xml:space="preserve">This is a summary of the second accident data point. </t>
+  </si>
+  <si>
+    <t>Accident Type</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Weather</t>
   </si>
 </sst>
 </file>
@@ -360,18 +369,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,10 +392,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -396,10 +409,13 @@
         <v>-86.4</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -410,6 +426,9 @@
         <v>-87</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ability to filter accidents by type
</commit_message>
<xml_diff>
--- a/src/img/traffic_data.xlsx
+++ b/src/img/traffic_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\Programming\Web Apps\2019 Accident Map Redesign\src\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2EB70D-31AC-403C-940B-5CDCE6C7EB58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7254EAB-2E9A-4C97-962A-D93EFFBB9986}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Record Number</t>
   </si>
@@ -39,19 +39,58 @@
     <t>Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a summary of the first accident data point. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a summary of the second accident data point. </t>
-  </si>
-  <si>
     <t>Accident Type</t>
   </si>
   <si>
-    <t>Animal</t>
-  </si>
-  <si>
     <t>Weather</t>
+  </si>
+  <si>
+    <t>V1 struck V2 while traveling west on W. Michigan Street</t>
+  </si>
+  <si>
+    <t>V1 struck pedestrian while they were crossing the street</t>
+  </si>
+  <si>
+    <t>V1 ran off the road due to ice on Michigan Street</t>
+  </si>
+  <si>
+    <t>V1 rearended V2 near Walnut St. and Barnhill Dr.</t>
+  </si>
+  <si>
+    <t>V1 struck V2 while turning left from University Blvd. to Wishard Blvd.</t>
+  </si>
+  <si>
+    <t>V1 struck two pedestrians as they crossed the street from Barnhill Garage to Carroll Stadium</t>
+  </si>
+  <si>
+    <t>V1 slid off the road due severse weather conditions (ice)</t>
+  </si>
+  <si>
+    <t>V1 rearended a bus stopped at the bus stop while picking up passengers. One passenger fell from the bus steps during the incident and was taken to Eskenazi Hospital as a precaution</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Roadway ID</t>
+  </si>
+  <si>
+    <t>W. Michigan Street</t>
+  </si>
+  <si>
+    <t>W. Walnut Street</t>
+  </si>
+  <si>
+    <t>Wishard Blvd.</t>
+  </si>
+  <si>
+    <t>University Blvd.</t>
+  </si>
+  <si>
+    <t>W. New York Street</t>
+  </si>
+  <si>
+    <t>Eskenazi Ave.</t>
   </si>
 </sst>
 </file>
@@ -369,19 +408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,44 +432,173 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>39.200000000000003</v>
+        <v>39.774537000000002</v>
       </c>
       <c r="C2">
-        <v>-86.4</v>
+        <v>-86.175438999999997</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>41</v>
+        <v>39.777228999999998</v>
       </c>
       <c r="C3">
-        <v>-87</v>
+        <v>-86.178774000000004</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>39.778146</v>
+      </c>
+      <c r="C4">
+        <v>-86.178729000000004</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>39.775764000000002</v>
+      </c>
+      <c r="C5">
+        <v>-86.186448999999996</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
+      </c>
+      <c r="B6">
+        <v>39.778677999999999</v>
+      </c>
+      <c r="C6">
+        <v>-86.174892999999997</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>39.771799000000001</v>
+      </c>
+      <c r="C7">
+        <v>-86.178151999999997</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>39.775593000000001</v>
+      </c>
+      <c r="C8">
+        <v>-86.183520000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>39.777782000000002</v>
+      </c>
+      <c r="C9">
+        <v>-86.182849000000004</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added icons for fatal accidents and formatting changes
</commit_message>
<xml_diff>
--- a/src/img/traffic_data.xlsx
+++ b/src/img/traffic_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\Programming\Web Apps\2019 Accident Map Redesign\src\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7254EAB-2E9A-4C97-962A-D93EFFBB9986}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D7ED9E-0D89-4049-9D10-F1279DBE9898}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Record Number</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Eskenazi Ave.</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Fatalities</t>
   </si>
 </sst>
 </file>
@@ -408,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,9 +428,10 @@
     <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,10 +448,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -455,13 +468,16 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -475,13 +491,16 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -497,11 +516,14 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -517,11 +539,14 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -535,13 +560,16 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -557,11 +585,14 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -577,11 +608,14 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -595,9 +629,12 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>